<commit_message>
updates in test files, and better error reporting
</commit_message>
<xml_diff>
--- a/tests/data/invalid.mirri.xlsx
+++ b/tests/data/invalid.mirri.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Locations" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Geographic origin" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Strains" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sexual states" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Genomic information" sheetId="4" state="visible" r:id="rId5"/>
@@ -479,7 +479,7 @@
     <t xml:space="preserve">Dual use</t>
   </si>
   <si>
-    <t xml:space="preserve">Quarantinein Europe</t>
+    <t xml:space="preserve">Quarantine in Europe</t>
   </si>
   <si>
     <t xml:space="preserve">Organism type</t>
@@ -25029,7 +25029,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K17" activeCellId="0" sqref="K17"/>
+      <selection pane="bottomRight" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>